<commit_message>
cambios de las fracciones
</commit_message>
<xml_diff>
--- a/xlsx/a69_f05UPPachuca.xlsx
+++ b/xlsx/a69_f05UPPachuca.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3er Trimestre 2022\Recepción de Información\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F8DD6A3-F292-4F0C-A3EF-DC1CA5882FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -19,12 +13,12 @@
   <definedNames>
     <definedName name="Hidden_114">Hidden_1!$A$1:$A$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
   <si>
     <t>44212</t>
   </si>
@@ -194,6 +188,9 @@
     <t>Descendente</t>
   </si>
   <si>
+    <t>Departamento de Evaluación y Estadistica (UPP)</t>
+  </si>
+  <si>
     <t>Incrementar la cobertura del sector educativo  en el nivel medio superior y superior para Estado de Hidalgo.</t>
   </si>
   <si>
@@ -203,9 +200,15 @@
     <t>Eficacia</t>
   </si>
   <si>
+    <t>Mide el porcentaje de atención a la demanda solicitada con respecto a los nuevos ingresos</t>
+  </si>
+  <si>
     <t>(Matricula de Nuevo Ingreso a primero (MTNI)/Solicitudes de Nuevo Ingreso a primero (STNI))x100</t>
   </si>
   <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
     <t>Anual</t>
   </si>
   <si>
@@ -215,21 +218,18 @@
     <t>Otorgar una oferta educativa de calidad a la población hidalguense.</t>
   </si>
   <si>
-    <t>Mide el porcentaje de atención a la demanda solicitada con respecto a los nuevos ingresos</t>
-  </si>
-  <si>
     <t>Porcentaje de Profesores de Tiempo Completo (PTC) que participan en los Cuerpos Académicos de la Universidad Politécnica de Pachuca.</t>
   </si>
   <si>
     <t>Mide la cantidad de Profesores de Tiempo Completo que participan en los Cuerpos Académicos en formación, en procesos de consolidación y consolidados, respecto al total de Profesores de Tiempo Completo adscritos a la Universidad Politécnica de Pachuca</t>
   </si>
   <si>
+    <t xml:space="preserve">(Total de Profesores de Tiempo Completo que participan en los cuerpos académicos en la UPP (TPTCCAUPP)/ Total de Profesores de Tiempo Completo adscritos a la UPP (TPTCUPP))x100 </t>
+  </si>
+  <si>
     <t>Profesores de Tiempo Completo</t>
   </si>
   <si>
-    <t xml:space="preserve">(Total de Profesores de Tiempo Completo que participan en los cuerpos académicos en la UPP (TPTCCAUPP)/ Total de Profesores de Tiempo Completo adscritos a la UPP (TPTCUPP))x100 </t>
-  </si>
-  <si>
     <t>Cuatrimestral</t>
   </si>
   <si>
@@ -245,9 +245,6 @@
     <t>(Población de 18 a 22 años  del ciclo escolar (P (18-22)n)/ Matricula Total (MTn))x100</t>
   </si>
   <si>
-    <t>Estudiante</t>
-  </si>
-  <si>
     <t>Ciclo escolar</t>
   </si>
   <si>
@@ -269,58 +266,52 @@
     <t>Universidad Politécnica de Pachuca</t>
   </si>
   <si>
+    <t>Impartir servicios educativos con suficiencia, calidad y relevancia, que garanticen el acceso a los niveles educativos en igualdad y con recursos destinados a programas de impacto que incidan en la mejora de las condiciones de bienestar de las personas.</t>
+  </si>
+  <si>
     <t>Porcentaje de proyectos concluidos de investigación o transferencia tecnológica</t>
   </si>
   <si>
     <t>Mide el porcentaje de proyectos concluidos de investigación con respecto al total de proyectos de investigación o transferencia tecnológica en los que participa la institución.</t>
   </si>
   <si>
+    <t xml:space="preserve">(Total de proyectos concluidos de investigación o transferencia tecnológica (TPITTCF) / Total de proyectos de investigación o transferencia de  tecnología en los que participa la institución (TPIT))x100 </t>
+  </si>
+  <si>
     <t>Proyecto</t>
   </si>
   <si>
     <t>Universidad Politécnica de Pachuca - Dirección de Innovación, Investigación y Posgrado</t>
   </si>
   <si>
+    <t>Fortalecer la personal docente de educación básica en el Estado</t>
+  </si>
+  <si>
+    <t>Porcentaje de personal docente que obtiene resultados aprobatorios en las evaluaciones</t>
+  </si>
+  <si>
+    <t>Mide el número de docentes que en las evaluaciones obtienen resultados aprobatorios</t>
+  </si>
+  <si>
+    <t>(Total de docentes con resultados aprobatorios (TDA)/ Total de docentes evaluados (TDE))x100</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
     <t>Universidad Politécnica de Pachuca - Secretaría Académica (UPP)</t>
   </si>
   <si>
-    <t>Fortalecer la personal docente de educación básica en el Estado</t>
-  </si>
-  <si>
-    <t>Porcentaje de personal docente que obtiene resultados aprobatorios en las evaluaciones</t>
-  </si>
-  <si>
-    <t>Mide el número de docentes que en las evaluaciones obtienen resultados aprobatorios</t>
-  </si>
-  <si>
-    <t>Docente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Total de proyectos concluidos de investigación o transferencia tecnológica (TPITTCF) / Total de proyectos de investigación o transferencia de  tecnología en los que participa la institución (TPIT))x100 </t>
-  </si>
-  <si>
-    <t>(Total de docentes con resultados aprobatorios (TDA)/ Total de docentes evaluados (TDE))x100</t>
-  </si>
-  <si>
-    <t>Impartir servicios educativos con suficiencia, calidad y relevancia, que garanticen el acceso a los niveles educativos en igualdad y con recursos destinados a programas de impacto que incidan en la mejora de las condiciones de bienestar de las personas.</t>
-  </si>
-  <si>
-    <t>Departamento de Evaluación y Estadísticas (UPP)</t>
-  </si>
-  <si>
     <t xml:space="preserve">
-Las metas ajustadas no fueron requeridas para este periodo. Las metas alcanzadas son del periodo abril-junio 2022. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Las metas ajustadas no fueron requeridas para este periodo.Las metas alcanzadas son del periodo abril-junio 2022. </t>
+Las metas ajustadas no fueron requeridas para este periodo.
+Metas alcanzadas son hasta septiembre 2022. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -341,6 +332,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -360,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -383,19 +381,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -409,14 +416,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,39 +456,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -513,7 +523,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,175 +567,199 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
-    <col min="8" max="8" width="35" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" customWidth="1"/>
-    <col min="10" max="10" width="31" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1"/>
-    <col min="13" max="13" width="35.140625" customWidth="1"/>
-    <col min="14" max="14" width="56" customWidth="1"/>
-    <col min="15" max="15" width="34" customWidth="1"/>
-    <col min="16" max="16" width="47.42578125" customWidth="1"/>
-    <col min="17" max="17" width="81.5703125" customWidth="1"/>
-    <col min="18" max="18" width="24" customWidth="1"/>
-    <col min="19" max="19" width="32" customWidth="1"/>
-    <col min="20" max="20" width="51.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="63.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
@@ -750,7 +784,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:20" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -761,11 +795,11 @@
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -829,7 +863,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -977,36 +1011,36 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>2022</v>
       </c>
-      <c r="B8" s="3">
-        <v>44743</v>
-      </c>
-      <c r="C8" s="3">
-        <v>44834</v>
+      <c r="B8" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44926</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="K8" s="5">
         <v>0.47</v>
@@ -1014,59 +1048,59 @@
       <c r="L8" s="4">
         <v>1400</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="O8" s="4" t="s">
+      <c r="M8" s="5"/>
+      <c r="N8" s="11">
+        <v>0.38</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>54</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R8" s="3">
-        <v>44844</v>
-      </c>
-      <c r="S8" s="3">
-        <v>44844</v>
-      </c>
-      <c r="T8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" s="2">
+        <v>44936</v>
+      </c>
+      <c r="S8" s="2">
+        <v>44936</v>
+      </c>
+      <c r="T8" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="240" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>2022</v>
       </c>
-      <c r="B9" s="3">
-        <v>44743</v>
-      </c>
-      <c r="C9" s="3">
-        <v>44834</v>
+      <c r="B9" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44926</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K9" s="5">
         <v>0.59</v>
@@ -1074,59 +1108,59 @@
       <c r="L9" s="4">
         <v>88</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="5">
+      <c r="M9" s="5"/>
+      <c r="N9" s="11">
         <v>0.57999999999999996</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="3" t="s">
         <v>54</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R9" s="3">
-        <v>44844</v>
-      </c>
-      <c r="S9" s="3">
-        <v>44844</v>
-      </c>
-      <c r="T9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" s="2">
+        <v>44936</v>
+      </c>
+      <c r="S9" s="2">
+        <v>44936</v>
+      </c>
+      <c r="T9" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>2022</v>
       </c>
-      <c r="B10" s="3">
-        <v>44743</v>
-      </c>
-      <c r="C10" s="3">
-        <v>44834</v>
+      <c r="B10" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44926</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K10" s="5">
         <v>0.72</v>
@@ -1134,59 +1168,59 @@
       <c r="L10" s="4">
         <v>3990</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="5">
+      <c r="M10" s="5"/>
+      <c r="N10" s="11">
         <v>0.72</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R10" s="3">
-        <v>44844</v>
-      </c>
-      <c r="S10" s="3">
-        <v>44844</v>
-      </c>
-      <c r="T10" s="9" t="s">
-        <v>95</v>
+        <v>64</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="2">
+        <v>44936</v>
+      </c>
+      <c r="S10" s="2">
+        <v>44936</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="240" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>2022</v>
       </c>
-      <c r="B11" s="3">
-        <v>44743</v>
-      </c>
-      <c r="C11" s="3">
-        <v>44834</v>
+      <c r="B11" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44926</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="I11" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="J11" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K11" s="5">
         <v>0.95</v>
@@ -1194,59 +1228,59 @@
       <c r="L11" s="4">
         <v>5</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="5">
-        <v>0.77</v>
-      </c>
-      <c r="O11" s="4" t="s">
+      <c r="M11" s="5"/>
+      <c r="N11" s="11">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>54</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R11" s="3">
-        <v>44844</v>
-      </c>
-      <c r="S11" s="3">
-        <v>44844</v>
-      </c>
-      <c r="T11" s="9" t="s">
-        <v>95</v>
+        <v>81</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R11" s="2">
+        <v>44936</v>
+      </c>
+      <c r="S11" s="2">
+        <v>44936</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>2022</v>
       </c>
-      <c r="B12" s="3">
-        <v>44743</v>
-      </c>
-      <c r="C12" s="3">
-        <v>44834</v>
+      <c r="B12" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44926</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>58</v>
+        <v>83</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>60</v>
+        <v>85</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="K12" s="5">
         <v>7.0000000000000007E-2</v>
@@ -1254,59 +1288,59 @@
       <c r="L12" s="4">
         <v>5</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="5">
+      <c r="M12" s="5"/>
+      <c r="N12" s="11">
         <v>0</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="3" t="s">
         <v>54</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R12" s="3">
-        <v>44844</v>
-      </c>
-      <c r="S12" s="3">
-        <v>44844</v>
-      </c>
-      <c r="T12" s="9" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R12" s="2">
+        <v>44936</v>
+      </c>
+      <c r="S12" s="2">
+        <v>44936</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>2022</v>
       </c>
-      <c r="B13" s="3">
-        <v>44743</v>
-      </c>
-      <c r="C13" s="3">
-        <v>44834</v>
+      <c r="B13" s="2">
+        <v>44835</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44926</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>89</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>89</v>
+      <c r="I13" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K13" s="5">
         <v>0.79</v>
@@ -1314,27 +1348,27 @@
       <c r="L13" s="4">
         <v>164</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="5">
-        <v>0.87</v>
-      </c>
-      <c r="O13" s="4" t="s">
+      <c r="M13" s="5"/>
+      <c r="N13" s="11">
+        <v>0.89</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>54</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="R13" s="3">
-        <v>44844</v>
-      </c>
-      <c r="S13" s="3">
-        <v>44844</v>
-      </c>
-      <c r="T13" s="9" t="s">
-        <v>95</v>
+      <c r="Q13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="R13" s="2">
+        <v>44936</v>
+      </c>
+      <c r="S13" s="2">
+        <v>44936</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1348,17 +1382,16 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O8:O57" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O8:O201">
       <formula1>Hidden_114</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>